<commit_message>
Added seminar paper, updated README, updated Delta Explanation
</commit_message>
<xml_diff>
--- a/Nussbaum2020_DeltaExplanation.xlsx
+++ b/Nussbaum2020_DeltaExplanation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nusjoh00/Desktop/Dropbox/Lehrveranstaltungen/20FS Lauer Machine Learning/Autorerkennung NT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johannes\Dropbox\Lehrveranstaltungen\20FS Lauer Machine Learning\Autorerkennung NT\authorship-attribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9088FF3-64CC-D64B-9851-499B298A4FAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CEBBB1-25B4-4083-A97F-2737F94BB154}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="1340" windowWidth="31840" windowHeight="19660" xr2:uid="{160738BD-9FA5-2346-A730-3B06B48EDAC5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{160738BD-9FA5-2346-A730-3B06B48EDAC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,39 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={B5D500E2-E2FF-4A4C-9CC2-40B7C956FDF3}</author>
+  </authors>
+  <commentList>
+    <comment ref="E71" authorId="0" shapeId="0" xr:uid="{B5D500E2-E2FF-4A4C-9CC2-40B7C956FDF3}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    wieso kommt der mean noch rein?</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="63">
   <si>
     <t>X</t>
   </si>
@@ -236,6 +263,9 @@
   <si>
     <t>This excel sheet is an appendix to a seminar paper. All files available at</t>
   </si>
+  <si>
+    <t>https://github.com/jnussbaum/authorship-attribution</t>
+  </si>
 </sst>
 </file>
 
@@ -244,7 +274,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -271,6 +301,20 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -449,10 +493,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -516,30 +561,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -555,9 +576,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1649,8 +1696,14 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Johannes Nussbaum" id="{FFB614C3-4AE9-44D0-A25C-5D4A4D827AA2}" userId="Johannes Nussbaum" providerId="None"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1944,80 +1997,93 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E71" dT="2021-01-22T22:12:12.72" personId="{FFB614C3-4AE9-44D0-A25C-5D4A4D827AA2}" id="{B5D500E2-E2FF-4A4C-9CC2-40B7C956FDF3}">
+    <text>wieso kommt der mean noch rein?</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0B8B6E-5404-204B-B0F6-6A6034643ACD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0B8B6E-5404-204B-B0F6-6A6034643ACD}">
   <dimension ref="A1:U128"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="4" width="6.83203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="11" width="6.83203125" customWidth="1"/>
-    <col min="15" max="18" width="7.1640625" customWidth="1"/>
+    <col min="2" max="4" width="6.796875" customWidth="1"/>
+    <col min="5" max="5" width="6.796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.296875" customWidth="1"/>
+    <col min="7" max="7" width="12.69921875" customWidth="1"/>
+    <col min="8" max="11" width="6.796875" customWidth="1"/>
+    <col min="15" max="18" width="7.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="41" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="56" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>"Document1 = ''"&amp;B16&amp;C16&amp;D16&amp;E16&amp;"''"</f>
         <v>Document1 = ''AABB''</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>"Document2 = ''"&amp;B17&amp;C17&amp;D17&amp;E17&amp;"''"</f>
         <v>Document2 = ''ABBC''</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>"Document3 = ''"&amp;B18&amp;C18&amp;D18&amp;E18&amp;"''"</f>
         <v>Document3 = ''CCCC''</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f>"Document4 = ''"&amp;B19&amp;C19&amp;D19&amp;E19&amp;"''"</f>
         <v>Document4 = ''D''</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>10</v>
       </c>
@@ -2034,7 +2100,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>11</v>
       </c>
@@ -2051,7 +2117,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
         <v>12</v>
       </c>
@@ -2068,7 +2134,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
         <v>13</v>
       </c>
@@ -2079,78 +2145,78 @@
       <c r="D19" s="10"/>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="29"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="29"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="29"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="36" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="51" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="43" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="26" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="26" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="26"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="26"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="26"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>28</v>
       </c>
       <c r="E33"/>
     </row>
-    <row r="34" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="35"/>
       <c r="B34" s="18" t="s">
         <v>19</v>
@@ -2165,7 +2231,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
         <v>10</v>
       </c>
@@ -2186,7 +2252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
         <v>11</v>
       </c>
@@ -2207,7 +2273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
         <v>12</v>
       </c>
@@ -2228,7 +2294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="14" t="s">
         <v>13</v>
       </c>
@@ -2249,55 +2315,55 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E40"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="40" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B42" s="40"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="40"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
-      <c r="C43" s="40"/>
-      <c r="D43" s="40"/>
-      <c r="E43" s="40"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="45" t="s">
+      <c r="B42" s="49"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="49"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="49"/>
+      <c r="E43" s="49"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="B44" s="45"/>
-      <c r="C44" s="45"/>
-      <c r="D44" s="45"/>
-      <c r="E44" s="45"/>
-    </row>
-    <row r="45" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="46"/>
-      <c r="B45" s="46"/>
-      <c r="C45" s="46"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="46"/>
-    </row>
-    <row r="46" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="54"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="54"/>
+    </row>
+    <row r="45" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="55"/>
+      <c r="B45" s="55"/>
+      <c r="C45" s="55"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="55"/>
+    </row>
+    <row r="46" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="35"/>
       <c r="B46" s="18" t="s">
         <v>19</v>
@@ -2311,11 +2377,11 @@
       <c r="E46" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F46" s="52" t="s">
+      <c r="F46" s="44" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>10</v>
       </c>
@@ -2335,12 +2401,12 @@
         <f>COUNTIF(B16:E16,"D")/COUNTIF(B16:E16,"*")</f>
         <v>0</v>
       </c>
-      <c r="F47" s="53">
+      <c r="F47" s="45">
         <f>SUM(B47:E47)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
         <v>11</v>
       </c>
@@ -2360,12 +2426,12 @@
         <f>COUNTIF(B17:E17,"D")/COUNTIF(B17:E17,"*")</f>
         <v>0</v>
       </c>
-      <c r="F48" s="54">
+      <c r="F48" s="46">
         <f t="shared" ref="F48:F50" si="0">SUM(B48:E48)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
         <v>12</v>
       </c>
@@ -2385,12 +2451,12 @@
         <f>COUNTIF(B18:E18,"D")/COUNTIF(B18:E18,"*")</f>
         <v>0</v>
       </c>
-      <c r="F49" s="54">
+      <c r="F49" s="46">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="14" t="s">
         <v>13</v>
       </c>
@@ -2410,12 +2476,12 @@
         <f>COUNTIF(B19:E19,"D")/COUNTIF(B19:E19,"*")</f>
         <v>1</v>
       </c>
-      <c r="F50" s="55">
+      <c r="F50" s="47">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="14" t="s">
         <v>18</v>
       </c>
@@ -2437,7 +2503,7 @@
       </c>
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="14" t="s">
         <v>27</v>
       </c>
@@ -2458,14 +2524,14 @@
         <v>0.4330127018922193</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="7"/>
       <c r="B53" s="27"/>
       <c r="C53" s="27"/>
       <c r="D53" s="27"/>
       <c r="E53" s="27"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="15" t="s">
         <v>34</v>
       </c>
@@ -2474,30 +2540,30 @@
       <c r="D54" s="27"/>
       <c r="E54" s="27"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="45" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="45"/>
-      <c r="C55" s="45"/>
-      <c r="D55" s="45"/>
-      <c r="E55" s="45"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="45"/>
-      <c r="B56" s="45"/>
-      <c r="C56" s="45"/>
-      <c r="D56" s="45"/>
-      <c r="E56" s="45"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="45"/>
-      <c r="B57" s="45"/>
-      <c r="C57" s="45"/>
-      <c r="D57" s="45"/>
-      <c r="E57" s="45"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B55" s="54"/>
+      <c r="C55" s="54"/>
+      <c r="D55" s="54"/>
+      <c r="E55" s="54"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="54"/>
+      <c r="B56" s="54"/>
+      <c r="C56" s="54"/>
+      <c r="D56" s="54"/>
+      <c r="E56" s="54"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" s="54"/>
+      <c r="B57" s="54"/>
+      <c r="C57" s="54"/>
+      <c r="D57" s="54"/>
+      <c r="E57" s="54"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="str">
         <f>A47&amp;" = point/vector ("&amp;B47&amp;" | "&amp;C47&amp;" | "&amp;D47&amp;" | "&amp;E47&amp;")"</f>
         <v>Document1 = point/vector (0.5 | 0.5 | 0 | 0)</v>
@@ -2514,7 +2580,7 @@
         <v>0.70710678118654757</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="str">
         <f>A48&amp;" = point/vector ("&amp;B48&amp;" | "&amp;C48&amp;" | "&amp;D48&amp;" | "&amp;E48&amp;")"</f>
         <v>Document2 = point/vector (0.25 | 0.5 | 0.25 | 0)</v>
@@ -2531,7 +2597,7 @@
         <v>0.61237243569579447</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="str">
         <f>A49&amp;" = point/vector ("&amp;B49&amp;" | "&amp;C49&amp;" | "&amp;D49&amp;" | "&amp;E49&amp;")"</f>
         <v>Document3 = point/vector (0 | 0 | 1 | 0)</v>
@@ -2548,7 +2614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="str">
         <f>A50&amp;" = point/vector ("&amp;B50&amp;" | "&amp;C50&amp;" | "&amp;D50&amp;" | "&amp;E50&amp;")"</f>
         <v>Document4 = point/vector (0 | 0 | 0 | 1)</v>
@@ -2565,35 +2631,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="7"/>
       <c r="B62" s="27"/>
       <c r="C62" s="27"/>
       <c r="D62" s="27"/>
       <c r="E62" s="27"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="7"/>
       <c r="B63" s="27"/>
       <c r="C63" s="27"/>
       <c r="D63" s="27"/>
       <c r="E63" s="27"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="7"/>
       <c r="B64" s="27"/>
       <c r="C64" s="27"/>
       <c r="D64" s="27"/>
       <c r="E64" s="27"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="7"/>
       <c r="B65" s="27"/>
       <c r="C65" s="27"/>
       <c r="D65" s="27"/>
       <c r="E65" s="27"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="15" t="s">
         <v>44</v>
       </c>
@@ -2602,47 +2668,47 @@
       </c>
       <c r="K66" s="1"/>
     </row>
-    <row r="67" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="39" t="s">
+    <row r="67" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="B67" s="39"/>
-      <c r="C67" s="39"/>
-      <c r="D67" s="39"/>
-      <c r="E67" s="39"/>
-      <c r="G67" s="39" t="s">
+      <c r="B67" s="52"/>
+      <c r="C67" s="52"/>
+      <c r="D67" s="52"/>
+      <c r="E67" s="52"/>
+      <c r="G67" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="H67" s="39"/>
-      <c r="I67" s="39"/>
-      <c r="J67" s="39"/>
-      <c r="K67" s="39"/>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A68" s="39"/>
-      <c r="B68" s="39"/>
-      <c r="C68" s="39"/>
-      <c r="D68" s="39"/>
-      <c r="E68" s="39"/>
-      <c r="G68" s="39"/>
-      <c r="H68" s="39"/>
-      <c r="I68" s="39"/>
-      <c r="J68" s="39"/>
-      <c r="K68" s="39"/>
-    </row>
-    <row r="69" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="44"/>
-      <c r="B69" s="44"/>
-      <c r="C69" s="44"/>
-      <c r="D69" s="44"/>
-      <c r="E69" s="44"/>
-      <c r="G69" s="44"/>
-      <c r="H69" s="44"/>
-      <c r="I69" s="44"/>
-      <c r="J69" s="44"/>
-      <c r="K69" s="44"/>
-    </row>
-    <row r="70" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H67" s="52"/>
+      <c r="I67" s="52"/>
+      <c r="J67" s="52"/>
+      <c r="K67" s="52"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A68" s="52"/>
+      <c r="B68" s="52"/>
+      <c r="C68" s="52"/>
+      <c r="D68" s="52"/>
+      <c r="E68" s="52"/>
+      <c r="G68" s="52"/>
+      <c r="H68" s="52"/>
+      <c r="I68" s="52"/>
+      <c r="J68" s="52"/>
+      <c r="K68" s="52"/>
+    </row>
+    <row r="69" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="53"/>
+      <c r="B69" s="53"/>
+      <c r="C69" s="53"/>
+      <c r="D69" s="53"/>
+      <c r="E69" s="53"/>
+      <c r="G69" s="53"/>
+      <c r="H69" s="53"/>
+      <c r="I69" s="53"/>
+      <c r="J69" s="53"/>
+      <c r="K69" s="53"/>
+    </row>
+    <row r="70" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="35"/>
       <c r="B70" s="18" t="s">
         <v>19</v>
@@ -2670,7 +2736,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="13" t="s">
         <v>10</v>
       </c>
@@ -2694,23 +2760,23 @@
         <v>10</v>
       </c>
       <c r="H71" s="27">
-        <f>ROUND(B47/$H58,1)</f>
+        <f t="shared" ref="H71:K74" si="1">ROUND(B47/$H58,1)</f>
         <v>0.7</v>
       </c>
       <c r="I71" s="27">
-        <f>ROUND(C47/$H58,1)</f>
+        <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
       <c r="J71" s="27">
-        <f>ROUND(D47/$H58,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K71" s="28">
-        <f>ROUND(E47/$H58,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="13" t="s">
         <v>11</v>
       </c>
@@ -2734,23 +2800,23 @@
         <v>11</v>
       </c>
       <c r="H72" s="27">
-        <f>ROUND(B48/$H59,1)</f>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
       <c r="I72" s="27">
-        <f>ROUND(C48/$H59,1)</f>
+        <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
       <c r="J72" s="27">
-        <f>ROUND(D48/$H59,1)</f>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
       <c r="K72" s="28">
-        <f>ROUND(E48/$H59,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="13" t="s">
         <v>12</v>
       </c>
@@ -2774,23 +2840,23 @@
         <v>12</v>
       </c>
       <c r="H73" s="27">
-        <f>ROUND(B49/$H60,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I73" s="27">
-        <f>ROUND(C49/$H60,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J73" s="27">
-        <f>ROUND(D49/$H60,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K73" s="28">
-        <f>ROUND(E49/$H60,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="14" t="s">
         <v>13</v>
       </c>
@@ -2814,23 +2880,23 @@
         <v>13</v>
       </c>
       <c r="H74" s="22">
-        <f>ROUND(B50/$H61,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I74" s="22">
-        <f>ROUND(C50/$H61,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J74" s="22">
-        <f>ROUND(D50/$H61,1)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K74" s="23">
-        <f>ROUND(E50/$H61,1)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="14" t="s">
         <v>18</v>
       </c>
@@ -2839,25 +2905,25 @@
         <v>0</v>
       </c>
       <c r="C75" s="24">
-        <f t="shared" ref="C75:E75" si="1">AVERAGE(C71:C74)</f>
+        <f t="shared" ref="C75:E75" si="2">AVERAGE(C71:C74)</f>
         <v>0</v>
       </c>
       <c r="D75" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.5000000000000022E-2</v>
       </c>
       <c r="E75" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-2.4999999999999967E-2</v>
       </c>
       <c r="F75" s="6"/>
       <c r="G75" s="4"/>
-      <c r="H75" s="47"/>
-      <c r="I75" s="47"/>
-      <c r="J75" s="47"/>
-      <c r="K75" s="50"/>
-    </row>
-    <row r="76" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H75" s="39"/>
+      <c r="I75" s="39"/>
+      <c r="J75" s="39"/>
+      <c r="K75" s="42"/>
+    </row>
+    <row r="76" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="14" t="s">
         <v>27</v>
       </c>
@@ -2866,25 +2932,25 @@
         <v>0.99498743710661997</v>
       </c>
       <c r="C76" s="24">
-        <f t="shared" ref="C76:E76" si="2">_xlfn.STDEV.P(C71:C74)</f>
+        <f t="shared" ref="C76:E76" si="3">_xlfn.STDEV.P(C71:C74)</f>
         <v>1</v>
       </c>
       <c r="D76" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0256095748383007</v>
       </c>
       <c r="E76" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.99592921435210446</v>
       </c>
       <c r="F76" s="26"/>
       <c r="G76" s="7"/>
-      <c r="H76" s="47"/>
-      <c r="I76" s="47"/>
-      <c r="J76" s="47"/>
-      <c r="K76" s="47"/>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H76" s="39"/>
+      <c r="I76" s="39"/>
+      <c r="J76" s="39"/>
+      <c r="K76" s="39"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="6"/>
       <c r="B77" s="37"/>
       <c r="C77" s="37"/>
@@ -2892,7 +2958,7 @@
       <c r="E77" s="37"/>
       <c r="F77" s="26"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="15" t="s">
         <v>34</v>
       </c>
@@ -2905,7 +2971,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="38" t="str">
         <f>A71&amp;" = point/vector ("&amp;B71&amp;" | "&amp;C71&amp;" | "&amp;D71&amp;" | "&amp;E71&amp;")"</f>
         <v>Document1 = point/vector (1.5 | 1 | -0.8 | -0.6)</v>
@@ -2920,7 +2986,7 @@
         <v>Document1 = point/vector (0.7 | 0.7 | 0 | 0)</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="38" t="str">
         <f>A72&amp;" = point/vector ("&amp;B72&amp;" | "&amp;C72&amp;" | "&amp;D72&amp;" | "&amp;E72&amp;")"</f>
         <v>Document2 = point/vector (0.3 | 1 | -0.2 | -0.6)</v>
@@ -2935,7 +3001,7 @@
         <v>Document2 = point/vector (0.4 | 0.8 | 0.4 | 0)</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A81" s="38" t="str">
         <f>A73&amp;" = point/vector ("&amp;B73&amp;" | "&amp;C73&amp;" | "&amp;D73&amp;" | "&amp;E73&amp;")"</f>
         <v>Document3 = point/vector (-0.9 | -1 | 1.7 | -0.6)</v>
@@ -2950,7 +3016,7 @@
         <v>Document3 = point/vector (0 | 0 | 1 | 0)</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A82" s="38" t="str">
         <f>A74&amp;" = point/vector ("&amp;B74&amp;" | "&amp;C74&amp;" | "&amp;D74&amp;" | "&amp;E74&amp;")"</f>
         <v>Document4 = point/vector (-0.9 | -1 | -0.8 | 1.7)</v>
@@ -2965,7 +3031,7 @@
         <v>Document4 = point/vector (0 | 0 | 0 | 1)</v>
       </c>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A83" s="38"/>
       <c r="B83" s="37"/>
       <c r="C83" s="37"/>
@@ -2974,7 +3040,7 @@
       <c r="F83" s="26"/>
       <c r="G83" s="38"/>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A84" s="38"/>
       <c r="B84" s="37"/>
       <c r="C84" s="37"/>
@@ -2983,7 +3049,7 @@
       <c r="F84" s="26"/>
       <c r="G84" s="38"/>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A85" s="38"/>
       <c r="B85" s="37"/>
       <c r="C85" s="37"/>
@@ -2992,7 +3058,7 @@
       <c r="F85" s="26"/>
       <c r="G85" s="38"/>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A86" s="38"/>
       <c r="B86" s="37"/>
       <c r="C86" s="37"/>
@@ -3001,7 +3067,7 @@
       <c r="F86" s="26"/>
       <c r="G86" s="38"/>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A87" s="6"/>
       <c r="B87" s="37"/>
       <c r="C87" s="37"/>
@@ -3020,106 +3086,106 @@
         <v>53</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A88" s="6"/>
       <c r="B88" s="37"/>
       <c r="C88" s="37"/>
       <c r="D88" s="37"/>
       <c r="E88" s="37"/>
       <c r="F88" s="26"/>
-      <c r="G88" s="41" t="s">
+      <c r="G88" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="H88" s="41"/>
-      <c r="I88" s="41"/>
-      <c r="J88" s="41"/>
-      <c r="K88" s="41"/>
-      <c r="N88" s="43" t="s">
+      <c r="H88" s="50"/>
+      <c r="I88" s="50"/>
+      <c r="J88" s="50"/>
+      <c r="K88" s="50"/>
+      <c r="N88" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="O88" s="43"/>
-      <c r="P88" s="43"/>
-      <c r="Q88" s="43"/>
-      <c r="R88" s="43"/>
-      <c r="S88" s="43"/>
-    </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="O88" s="48"/>
+      <c r="P88" s="48"/>
+      <c r="Q88" s="48"/>
+      <c r="R88" s="48"/>
+      <c r="S88" s="48"/>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A89" s="6"/>
       <c r="B89" s="37"/>
       <c r="C89" s="37"/>
       <c r="D89" s="37"/>
       <c r="E89" s="37"/>
       <c r="F89" s="26"/>
-      <c r="G89" s="41"/>
-      <c r="H89" s="41"/>
-      <c r="I89" s="41"/>
-      <c r="J89" s="41"/>
-      <c r="K89" s="41"/>
-      <c r="N89" s="43"/>
-      <c r="O89" s="43"/>
-      <c r="P89" s="43"/>
-      <c r="Q89" s="43"/>
-      <c r="R89" s="43"/>
-      <c r="S89" s="43"/>
-    </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="G89" s="50"/>
+      <c r="H89" s="50"/>
+      <c r="I89" s="50"/>
+      <c r="J89" s="50"/>
+      <c r="K89" s="50"/>
+      <c r="N89" s="48"/>
+      <c r="O89" s="48"/>
+      <c r="P89" s="48"/>
+      <c r="Q89" s="48"/>
+      <c r="R89" s="48"/>
+      <c r="S89" s="48"/>
+    </row>
+    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A90" s="6"/>
       <c r="B90" s="37"/>
       <c r="C90" s="37"/>
       <c r="D90" s="37"/>
       <c r="E90" s="37"/>
       <c r="F90" s="26"/>
-      <c r="G90" s="41"/>
-      <c r="H90" s="41"/>
-      <c r="I90" s="41"/>
-      <c r="J90" s="41"/>
-      <c r="K90" s="41"/>
-      <c r="N90" s="43"/>
-      <c r="O90" s="43"/>
-      <c r="P90" s="43"/>
-      <c r="Q90" s="43"/>
-      <c r="R90" s="43"/>
-      <c r="S90" s="43"/>
-    </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="G90" s="50"/>
+      <c r="H90" s="50"/>
+      <c r="I90" s="50"/>
+      <c r="J90" s="50"/>
+      <c r="K90" s="50"/>
+      <c r="N90" s="48"/>
+      <c r="O90" s="48"/>
+      <c r="P90" s="48"/>
+      <c r="Q90" s="48"/>
+      <c r="R90" s="48"/>
+      <c r="S90" s="48"/>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A91" s="6"/>
       <c r="B91" s="37"/>
       <c r="C91" s="37"/>
       <c r="D91" s="37"/>
       <c r="E91" s="37"/>
       <c r="F91" s="26"/>
-      <c r="G91" s="41"/>
-      <c r="H91" s="41"/>
-      <c r="I91" s="41"/>
-      <c r="J91" s="41"/>
-      <c r="K91" s="41"/>
-      <c r="N91" s="43"/>
-      <c r="O91" s="43"/>
-      <c r="P91" s="43"/>
-      <c r="Q91" s="43"/>
-      <c r="R91" s="43"/>
-      <c r="S91" s="43"/>
-    </row>
-    <row r="92" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G91" s="50"/>
+      <c r="H91" s="50"/>
+      <c r="I91" s="50"/>
+      <c r="J91" s="50"/>
+      <c r="K91" s="50"/>
+      <c r="N91" s="48"/>
+      <c r="O91" s="48"/>
+      <c r="P91" s="48"/>
+      <c r="Q91" s="48"/>
+      <c r="R91" s="48"/>
+      <c r="S91" s="48"/>
+    </row>
+    <row r="92" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="6"/>
       <c r="B92" s="37"/>
       <c r="C92" s="37"/>
       <c r="D92" s="37"/>
       <c r="E92" s="37"/>
       <c r="F92" s="26"/>
-      <c r="G92" s="42"/>
-      <c r="H92" s="42"/>
-      <c r="I92" s="42"/>
-      <c r="J92" s="42"/>
-      <c r="K92" s="42"/>
-      <c r="N92" s="43"/>
-      <c r="O92" s="43"/>
-      <c r="P92" s="43"/>
-      <c r="Q92" s="43"/>
-      <c r="R92" s="43"/>
-      <c r="S92" s="43"/>
-    </row>
-    <row r="93" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G92" s="51"/>
+      <c r="H92" s="51"/>
+      <c r="I92" s="51"/>
+      <c r="J92" s="51"/>
+      <c r="K92" s="51"/>
+      <c r="N92" s="48"/>
+      <c r="O92" s="48"/>
+      <c r="P92" s="48"/>
+      <c r="Q92" s="48"/>
+      <c r="R92" s="48"/>
+      <c r="S92" s="48"/>
+    </row>
+    <row r="93" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="6"/>
       <c r="B93" s="37"/>
       <c r="C93" s="37"/>
@@ -3153,7 +3219,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A94" s="6"/>
       <c r="B94" s="37"/>
       <c r="C94" s="37"/>
@@ -3193,7 +3259,7 @@
         <v>1.4071247279470289</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A95" s="6"/>
       <c r="B95" s="37"/>
       <c r="C95" s="37"/>
@@ -3233,7 +3299,7 @@
         <v>1.4000000000000001</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A96" s="6"/>
       <c r="B96" s="37"/>
       <c r="C96" s="37"/>
@@ -3273,8 +3339,8 @@
         <v>1.4142135623730951</v>
       </c>
     </row>
-    <row r="97" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="48"/>
+    <row r="97" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="40"/>
       <c r="B97" s="37"/>
       <c r="C97" s="37"/>
       <c r="D97" s="37"/>
@@ -3313,7 +3379,7 @@
       </c>
       <c r="R97" s="23"/>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A98" s="26"/>
       <c r="B98" s="37"/>
       <c r="C98" s="37"/>
@@ -3326,7 +3392,7 @@
       <c r="J98" s="27"/>
       <c r="K98" s="27"/>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A99" s="26"/>
       <c r="B99" s="37"/>
       <c r="C99" s="37"/>
@@ -3339,7 +3405,7 @@
       <c r="J99" s="27"/>
       <c r="K99" s="27"/>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A100" s="26"/>
       <c r="B100" s="37"/>
       <c r="C100" s="37"/>
@@ -3352,7 +3418,7 @@
       <c r="J100" s="27"/>
       <c r="K100" s="27"/>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -3360,7 +3426,7 @@
       <c r="E101" s="7"/>
       <c r="F101" s="26"/>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A102" s="15" t="s">
         <v>48</v>
       </c>
@@ -3373,81 +3439,81 @@
         <v>50</v>
       </c>
     </row>
-    <row r="103" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="41" t="s">
+    <row r="103" spans="1:18" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="B103" s="41"/>
-      <c r="C103" s="41"/>
-      <c r="D103" s="41"/>
-      <c r="E103" s="41"/>
+      <c r="B103" s="50"/>
+      <c r="C103" s="50"/>
+      <c r="D103" s="50"/>
+      <c r="E103" s="50"/>
       <c r="F103" s="26"/>
-      <c r="G103" s="43" t="s">
+      <c r="G103" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="H103" s="43"/>
-      <c r="I103" s="43"/>
-      <c r="J103" s="43"/>
-      <c r="K103" s="43"/>
-      <c r="L103" s="43"/>
-    </row>
-    <row r="104" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="41"/>
-      <c r="B104" s="41"/>
-      <c r="C104" s="41"/>
-      <c r="D104" s="41"/>
-      <c r="E104" s="41"/>
+      <c r="H103" s="48"/>
+      <c r="I103" s="48"/>
+      <c r="J103" s="48"/>
+      <c r="K103" s="48"/>
+      <c r="L103" s="48"/>
+    </row>
+    <row r="104" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="50"/>
+      <c r="B104" s="50"/>
+      <c r="C104" s="50"/>
+      <c r="D104" s="50"/>
+      <c r="E104" s="50"/>
       <c r="F104" s="26"/>
-      <c r="G104" s="43"/>
-      <c r="H104" s="43"/>
-      <c r="I104" s="43"/>
-      <c r="J104" s="43"/>
-      <c r="K104" s="43"/>
-      <c r="L104" s="43"/>
-    </row>
-    <row r="105" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="41"/>
-      <c r="B105" s="41"/>
-      <c r="C105" s="41"/>
-      <c r="D105" s="41"/>
-      <c r="E105" s="41"/>
+      <c r="G104" s="48"/>
+      <c r="H104" s="48"/>
+      <c r="I104" s="48"/>
+      <c r="J104" s="48"/>
+      <c r="K104" s="48"/>
+      <c r="L104" s="48"/>
+    </row>
+    <row r="105" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="50"/>
+      <c r="B105" s="50"/>
+      <c r="C105" s="50"/>
+      <c r="D105" s="50"/>
+      <c r="E105" s="50"/>
       <c r="F105" s="26"/>
-      <c r="G105" s="43"/>
-      <c r="H105" s="43"/>
-      <c r="I105" s="43"/>
-      <c r="J105" s="43"/>
-      <c r="K105" s="43"/>
-      <c r="L105" s="43"/>
-    </row>
-    <row r="106" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="41"/>
-      <c r="B106" s="41"/>
-      <c r="C106" s="41"/>
-      <c r="D106" s="41"/>
-      <c r="E106" s="41"/>
+      <c r="G105" s="48"/>
+      <c r="H105" s="48"/>
+      <c r="I105" s="48"/>
+      <c r="J105" s="48"/>
+      <c r="K105" s="48"/>
+      <c r="L105" s="48"/>
+    </row>
+    <row r="106" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="50"/>
+      <c r="B106" s="50"/>
+      <c r="C106" s="50"/>
+      <c r="D106" s="50"/>
+      <c r="E106" s="50"/>
       <c r="F106" s="26"/>
-      <c r="G106" s="43"/>
-      <c r="H106" s="43"/>
-      <c r="I106" s="43"/>
-      <c r="J106" s="43"/>
-      <c r="K106" s="43"/>
-      <c r="L106" s="43"/>
-    </row>
-    <row r="107" spans="1:18" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="42"/>
-      <c r="B107" s="42"/>
-      <c r="C107" s="42"/>
-      <c r="D107" s="42"/>
-      <c r="E107" s="42"/>
+      <c r="G106" s="48"/>
+      <c r="H106" s="48"/>
+      <c r="I106" s="48"/>
+      <c r="J106" s="48"/>
+      <c r="K106" s="48"/>
+      <c r="L106" s="48"/>
+    </row>
+    <row r="107" spans="1:18" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A107" s="51"/>
+      <c r="B107" s="51"/>
+      <c r="C107" s="51"/>
+      <c r="D107" s="51"/>
+      <c r="E107" s="51"/>
       <c r="F107" s="26"/>
-      <c r="G107" s="43"/>
-      <c r="H107" s="43"/>
-      <c r="I107" s="43"/>
-      <c r="J107" s="43"/>
-      <c r="K107" s="43"/>
-      <c r="L107" s="43"/>
-    </row>
-    <row r="108" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G107" s="48"/>
+      <c r="H107" s="48"/>
+      <c r="I107" s="48"/>
+      <c r="J107" s="48"/>
+      <c r="K107" s="48"/>
+      <c r="L107" s="48"/>
+    </row>
+    <row r="108" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="34"/>
       <c r="B108" s="32" t="s">
         <v>23</v>
@@ -3476,7 +3542,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A109" s="13" t="s">
         <v>23</v>
       </c>
@@ -3511,7 +3577,7 @@
         <v>3.8794329482541645</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A110" s="13" t="s">
         <v>24</v>
       </c>
@@ -3546,7 +3612,7 @@
         <v>3.3301651610693423</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A111" s="13" t="s">
         <v>25</v>
       </c>
@@ -3581,7 +3647,7 @@
         <v>3.3970575502926055</v>
       </c>
     </row>
-    <row r="112" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="14" t="s">
         <v>26</v>
       </c>
@@ -3616,7 +3682,7 @@
       </c>
       <c r="K112" s="23"/>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F113" s="26"/>
       <c r="G113" s="7"/>
       <c r="H113" s="30"/>
@@ -3624,53 +3690,53 @@
       <c r="J113" s="27"/>
       <c r="K113" s="27"/>
     </row>
-    <row r="114" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="41" t="s">
+    <row r="114" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="B114" s="41"/>
-      <c r="C114" s="41"/>
-      <c r="D114" s="41"/>
-      <c r="E114" s="41"/>
+      <c r="B114" s="50"/>
+      <c r="C114" s="50"/>
+      <c r="D114" s="50"/>
+      <c r="E114" s="50"/>
       <c r="F114" s="26"/>
-      <c r="G114" s="39" t="s">
+      <c r="G114" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="H114" s="39"/>
-      <c r="I114" s="39"/>
-      <c r="J114" s="39"/>
-      <c r="K114" s="39"/>
-      <c r="L114" s="39"/>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A115" s="41"/>
-      <c r="B115" s="41"/>
-      <c r="C115" s="41"/>
-      <c r="D115" s="41"/>
-      <c r="E115" s="41"/>
+      <c r="H114" s="52"/>
+      <c r="I114" s="52"/>
+      <c r="J114" s="52"/>
+      <c r="K114" s="52"/>
+      <c r="L114" s="52"/>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A115" s="50"/>
+      <c r="B115" s="50"/>
+      <c r="C115" s="50"/>
+      <c r="D115" s="50"/>
+      <c r="E115" s="50"/>
       <c r="F115" s="26"/>
-      <c r="G115" s="39"/>
-      <c r="H115" s="39"/>
-      <c r="I115" s="39"/>
-      <c r="J115" s="39"/>
-      <c r="K115" s="39"/>
-      <c r="L115" s="39"/>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A116" s="41"/>
-      <c r="B116" s="41"/>
-      <c r="C116" s="41"/>
-      <c r="D116" s="41"/>
-      <c r="E116" s="41"/>
+      <c r="G115" s="52"/>
+      <c r="H115" s="52"/>
+      <c r="I115" s="52"/>
+      <c r="J115" s="52"/>
+      <c r="K115" s="52"/>
+      <c r="L115" s="52"/>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A116" s="50"/>
+      <c r="B116" s="50"/>
+      <c r="C116" s="50"/>
+      <c r="D116" s="50"/>
+      <c r="E116" s="50"/>
       <c r="F116" s="26"/>
-      <c r="G116" s="39"/>
-      <c r="H116" s="39"/>
-      <c r="I116" s="39"/>
-      <c r="J116" s="39"/>
-      <c r="K116" s="39"/>
-      <c r="L116" s="39"/>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G116" s="52"/>
+      <c r="H116" s="52"/>
+      <c r="I116" s="52"/>
+      <c r="J116" s="52"/>
+      <c r="K116" s="52"/>
+      <c r="L116" s="52"/>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F117" s="26"/>
       <c r="G117" s="7"/>
       <c r="H117" s="30"/>
@@ -3678,7 +3744,7 @@
       <c r="J117" s="27"/>
       <c r="K117" s="27"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" s="15" t="s">
         <v>41</v>
       </c>
@@ -3689,7 +3755,7 @@
       <c r="J118" s="27"/>
       <c r="K118" s="27"/>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>42</v>
       </c>
@@ -3700,7 +3766,7 @@
       <c r="J119" s="27"/>
       <c r="K119" s="27"/>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>43</v>
       </c>
@@ -3711,7 +3777,7 @@
       <c r="J120" s="27"/>
       <c r="K120" s="27"/>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>54</v>
       </c>
@@ -3722,7 +3788,7 @@
       <c r="J121" s="27"/>
       <c r="K121" s="27"/>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F122" s="26"/>
       <c r="G122" s="7"/>
       <c r="H122" s="30"/>
@@ -3730,7 +3796,7 @@
       <c r="J122" s="27"/>
       <c r="K122" s="27"/>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
@@ -3738,7 +3804,7 @@
       <c r="E123" s="7"/>
       <c r="F123" s="26"/>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
@@ -3746,7 +3812,7 @@
       <c r="E124" s="7"/>
       <c r="F124" s="26"/>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" s="7"/>
       <c r="B125" s="7"/>
       <c r="C125" s="7"/>
@@ -3754,7 +3820,7 @@
       <c r="E125" s="7"/>
       <c r="F125" s="26"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126" s="7"/>
       <c r="B126" s="7"/>
       <c r="C126" s="7"/>
@@ -3762,7 +3828,7 @@
       <c r="E126" s="7"/>
       <c r="F126" s="26"/>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127" s="7"/>
       <c r="B127" s="7"/>
       <c r="C127" s="7"/>
@@ -3770,7 +3836,7 @@
       <c r="E127" s="7"/>
       <c r="F127" s="26"/>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" s="7"/>
       <c r="B128" s="7"/>
       <c r="C128" s="7"/>
@@ -3792,8 +3858,12 @@
     <mergeCell ref="A55:E57"/>
     <mergeCell ref="G88:K92"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1" xr:uid="{02D28814-3A1A-4611-93A8-0BC731B16ED6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -3805,9 +3875,9 @@
       <selection sqref="A1:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3827,7 +3897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3835,7 +3905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -3843,7 +3913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -3851,7 +3921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3859,7 +3929,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>

</xml_diff>